<commit_message>
Added ability to show classes on Sat and Sun. Added schedule bottom area
</commit_message>
<xml_diff>
--- a/actualSchedule.xlsx
+++ b/actualSchedule.xlsx
@@ -12,108 +12,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="50">
-  <si>
-    <t>6:00AM</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="53">
+  <si>
+    <t>6:00</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>6:30AM</t>
-  </si>
-  <si>
-    <t>7:00AM</t>
-  </si>
-  <si>
-    <t>7:30AM</t>
-  </si>
-  <si>
-    <t>8:00AM</t>
-  </si>
-  <si>
-    <t>8:30AM</t>
-  </si>
-  <si>
-    <t>9:00AM</t>
-  </si>
-  <si>
-    <t>9:30AM</t>
-  </si>
-  <si>
-    <t>10:00AM</t>
-  </si>
-  <si>
-    <t>10:30AM</t>
-  </si>
-  <si>
-    <t>11:00AM</t>
-  </si>
-  <si>
-    <t>11:30AM</t>
-  </si>
-  <si>
-    <t>12:00PM</t>
-  </si>
-  <si>
-    <t>12:30PM</t>
-  </si>
-  <si>
-    <t>1:00PM</t>
-  </si>
-  <si>
-    <t>1:30PM</t>
-  </si>
-  <si>
-    <t>2:00PM</t>
-  </si>
-  <si>
-    <t>2:30PM</t>
-  </si>
-  <si>
-    <t>3:00PM</t>
-  </si>
-  <si>
-    <t>3:30PM</t>
-  </si>
-  <si>
-    <t>4:00PM</t>
-  </si>
-  <si>
-    <t>4:30PM</t>
-  </si>
-  <si>
-    <t>5:00PM</t>
-  </si>
-  <si>
-    <t>5:30PM</t>
-  </si>
-  <si>
-    <t>6:00PM</t>
-  </si>
-  <si>
-    <t>6:30PM</t>
-  </si>
-  <si>
-    <t>7:00PM</t>
-  </si>
-  <si>
-    <t>7:30PM</t>
-  </si>
-  <si>
-    <t>8:00PM</t>
-  </si>
-  <si>
-    <t>8:30PM</t>
-  </si>
-  <si>
-    <t>9:00PM</t>
-  </si>
-  <si>
-    <t>9:30PM</t>
-  </si>
-  <si>
-    <t>10:00PM</t>
+    <t>6:30</t>
+  </si>
+  <si>
+    <t>7:00</t>
+  </si>
+  <si>
+    <t>7:30</t>
+  </si>
+  <si>
+    <t>8:00</t>
+  </si>
+  <si>
+    <t>8:30</t>
+  </si>
+  <si>
+    <t>9:00</t>
+  </si>
+  <si>
+    <t>9:30</t>
+  </si>
+  <si>
+    <t>10:00</t>
+  </si>
+  <si>
+    <t>10:30</t>
+  </si>
+  <si>
+    <t>11:00</t>
+  </si>
+  <si>
+    <t>11:30</t>
+  </si>
+  <si>
+    <t>12:00</t>
+  </si>
+  <si>
+    <t>12:30</t>
+  </si>
+  <si>
+    <t>13:00</t>
+  </si>
+  <si>
+    <t>13:30</t>
+  </si>
+  <si>
+    <t>14:00</t>
+  </si>
+  <si>
+    <t>14:30</t>
+  </si>
+  <si>
+    <t>15:00</t>
+  </si>
+  <si>
+    <t>15:30</t>
+  </si>
+  <si>
+    <t>16:00</t>
+  </si>
+  <si>
+    <t>16:30</t>
+  </si>
+  <si>
+    <t>17:00</t>
+  </si>
+  <si>
+    <t>17:30</t>
+  </si>
+  <si>
+    <t>18:00</t>
+  </si>
+  <si>
+    <t>18:30</t>
+  </si>
+  <si>
+    <t>19:00</t>
+  </si>
+  <si>
+    <t>19:30</t>
+  </si>
+  <si>
+    <t>20:00</t>
+  </si>
+  <si>
+    <t>20:30</t>
+  </si>
+  <si>
+    <t>21:00</t>
+  </si>
+  <si>
+    <t>21:30</t>
+  </si>
+  <si>
+    <t>22:00</t>
   </si>
   <si>
     <t>Monday</t>
@@ -162,6 +162,15 @@
   </si>
   <si>
     <t>Fortune 500 Club  LAB  7:00PM - 9:00PM  Hitchcock 131</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Vincente</t>
+  </si>
+  <si>
+    <t>Catherine</t>
   </si>
 </sst>
 </file>
@@ -199,6 +208,21 @@
       </patternFill>
     </fill>
     <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="48"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="46"/>
+      </patternFill>
+    </fill>
+    <fill>
       <patternFill/>
     </fill>
     <fill>
@@ -215,17 +239,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="48"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="48"/>
         <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
       </patternFill>
     </fill>
     <fill>
@@ -237,16 +251,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="46"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="46"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="97">
+  <borders count="119">
     <border>
       <left/>
       <right/>
@@ -1212,11 +1221,214 @@
         <color indexed="8"/>
       </bottom>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right/>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom>
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right>
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <right style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium"/>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="true" horizontal="center"/>
@@ -1233,86 +1445,86 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="true">
       <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="bottom" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="7" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="11" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="11" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="21" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="27" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="31" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="42" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="46" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="51" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
-      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="57" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="21" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="27" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="66" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="36" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="72" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="42" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="76" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="46" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="81" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="51" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="true">
-      <alignment wrapText="true" horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="57" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="61" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="66" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="72" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="76" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="81" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
@@ -1322,7 +1534,7 @@
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="86" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="86" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1330,7 +1542,47 @@
       <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="96" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="96" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="101" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="101" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="101" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="101" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="106" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="106" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="106" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="106" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="center" vertical="center" indent="0" textRotation="0" wrapText="true"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="112" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
+      <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="118" xfId="0" applyBorder="true" applyNumberFormat="true" applyFill="true" applyFont="true">
       <alignment horizontal="general" vertical="bottom" indent="0" textRotation="0" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -1370,301 +1622,301 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="B1" t="s" s="6">
+      <c r="B1" t="s" s="9">
         <v>34</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" t="s" s="6">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" t="s" s="9">
         <v>35</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" t="s" s="6">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" t="s" s="6">
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" t="s" s="9">
         <v>37</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" t="s" s="6">
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" t="s" s="9">
         <v>38</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" t="s" s="6">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" t="s" s="9">
         <v>39</v>
       </c>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" t="s" s="6">
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" t="s" s="9">
         <v>40</v>
       </c>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B2"/>
-      <c r="D2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="M2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="S2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="D2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="V2" s="11"/>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3"/>
-      <c r="D3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="M3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="S3" s="8"/>
-      <c r="V3" s="8"/>
+      <c r="D3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="V3" s="11"/>
     </row>
     <row r="4">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="P4" s="8"/>
-      <c r="S4" s="8"/>
-      <c r="V4" s="8"/>
+      <c r="D4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="P4" s="11"/>
+      <c r="S4" s="11"/>
+      <c r="V4" s="11"/>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="M5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="S5" s="8"/>
-      <c r="V5" s="8"/>
+      <c r="D5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="P5" s="11"/>
+      <c r="S5" s="11"/>
+      <c r="V5" s="11"/>
     </row>
     <row r="6">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="V6" s="8"/>
+      <c r="D6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="P6" s="11"/>
+      <c r="S6" s="11"/>
+      <c r="V6" s="11"/>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="M7" s="8"/>
-      <c r="P7" s="8"/>
-      <c r="S7" s="8"/>
-      <c r="V7" s="8"/>
+      <c r="D7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="P7" s="11"/>
+      <c r="S7" s="11"/>
+      <c r="V7" s="11"/>
     </row>
     <row r="8">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="M8" s="8"/>
-      <c r="P8" s="8"/>
-      <c r="S8" s="8"/>
-      <c r="V8" s="8"/>
+      <c r="D8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="P8" s="11"/>
+      <c r="S8" s="11"/>
+      <c r="V8" s="11"/>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="M9" s="8"/>
-      <c r="P9" s="8"/>
-      <c r="S9" s="8"/>
-      <c r="V9" s="8"/>
+      <c r="D9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="P9" s="11"/>
+      <c r="S9" s="11"/>
+      <c r="V9" s="11"/>
     </row>
     <row r="10">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="P10" s="8"/>
-      <c r="S10" s="8"/>
-      <c r="V10" s="8"/>
+      <c r="D10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="V10" s="11"/>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="M11" s="8"/>
-      <c r="P11" s="8"/>
-      <c r="S11" s="8"/>
-      <c r="V11" s="8"/>
+      <c r="D11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="P11" s="11"/>
+      <c r="S11" s="11"/>
+      <c r="V11" s="11"/>
     </row>
     <row r="12">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="M12" s="8"/>
-      <c r="P12" s="8"/>
-      <c r="S12" s="8"/>
-      <c r="V12" s="8"/>
+      <c r="D12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="P12" s="11"/>
+      <c r="S12" s="11"/>
+      <c r="V12" s="11"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="S13" s="8"/>
-      <c r="V13" s="8"/>
+      <c r="D13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="J13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="P13" s="11"/>
+      <c r="S13" s="11"/>
+      <c r="V13" s="11"/>
     </row>
     <row r="14">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="I14" s="23" t="s">
+      <c r="D14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="I14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="O14" s="23" t="s">
+      <c r="J14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="O14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="P14" s="8"/>
-      <c r="S14" s="8"/>
-      <c r="V14" s="8"/>
+      <c r="P14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="V14" s="11"/>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="O15" s="24"/>
-      <c r="P15" s="8"/>
-      <c r="S15" s="8"/>
-      <c r="V15" s="8"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="O15" s="25"/>
+      <c r="P15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="V15" s="11"/>
     </row>
     <row r="16">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="24"/>
-      <c r="D16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="O16" s="24"/>
-      <c r="P16" s="8"/>
-      <c r="S16" s="8"/>
-      <c r="V16" s="8"/>
+      <c r="C16" s="25"/>
+      <c r="D16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="11"/>
+      <c r="S16" s="11"/>
+      <c r="V16" s="11"/>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C17" s="25"/>
-      <c r="D17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="O17" s="25"/>
-      <c r="P17" s="8"/>
-      <c r="S17" s="8"/>
-      <c r="V17" s="8"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="11"/>
+      <c r="M17" s="11"/>
+      <c r="O17" s="26"/>
+      <c r="P17" s="11"/>
+      <c r="S17" s="11"/>
+      <c r="V17" s="11"/>
     </row>
     <row r="18">
       <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="M18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="S18" s="8"/>
-      <c r="V18" s="8"/>
+      <c r="D18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="J18" s="11"/>
+      <c r="M18" s="11"/>
+      <c r="P18" s="11"/>
+      <c r="S18" s="11"/>
+      <c r="V18" s="11"/>
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="S19" s="8"/>
-      <c r="V19" s="8"/>
+      <c r="D19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="J19" s="11"/>
+      <c r="M19" s="11"/>
+      <c r="P19" s="11"/>
+      <c r="S19" s="11"/>
+      <c r="V19" s="11"/>
     </row>
     <row r="20">
       <c r="A20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="G20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="V20" s="8"/>
+      <c r="D20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="M20" s="11"/>
+      <c r="P20" s="11"/>
+      <c r="S20" s="11"/>
+      <c r="V20" s="11"/>
     </row>
     <row r="21">
       <c r="A21" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="M21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="V21" s="8"/>
+      <c r="D21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="J21" s="11"/>
+      <c r="M21" s="11"/>
+      <c r="P21" s="11"/>
+      <c r="S21" s="11"/>
+      <c r="V21" s="11"/>
     </row>
     <row r="22">
       <c r="A22" s="3" t="s">
@@ -1676,13 +1928,13 @@
       <c r="G22" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="J22" s="8"/>
+      <c r="J22" s="11"/>
       <c r="M22" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="P22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="V22" s="8"/>
+      <c r="P22" s="11"/>
+      <c r="S22" s="11"/>
+      <c r="V22" s="11"/>
     </row>
     <row r="23">
       <c r="A23" s="2" t="s">
@@ -1690,11 +1942,11 @@
       </c>
       <c r="D23" s="29"/>
       <c r="G23" s="29"/>
-      <c r="J23" s="8"/>
+      <c r="J23" s="11"/>
       <c r="M23" s="29"/>
-      <c r="P23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="V23" s="8"/>
+      <c r="P23" s="11"/>
+      <c r="S23" s="11"/>
+      <c r="V23" s="11"/>
     </row>
     <row r="24">
       <c r="A24" s="3" t="s">
@@ -1702,11 +1954,11 @@
       </c>
       <c r="D24" s="29"/>
       <c r="G24" s="29"/>
-      <c r="J24" s="8"/>
+      <c r="J24" s="11"/>
       <c r="M24" s="29"/>
-      <c r="P24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="V24" s="8"/>
+      <c r="P24" s="11"/>
+      <c r="S24" s="11"/>
+      <c r="V24" s="11"/>
     </row>
     <row r="25">
       <c r="A25" s="2" t="s">
@@ -1714,263 +1966,263 @@
       </c>
       <c r="D25" s="31"/>
       <c r="G25" s="31"/>
-      <c r="J25" s="8"/>
+      <c r="J25" s="11"/>
       <c r="M25" s="31"/>
-      <c r="P25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="V25" s="8"/>
+      <c r="P25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="V25" s="11"/>
     </row>
     <row r="26">
       <c r="A26" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="M26" s="8"/>
-      <c r="P26" s="8"/>
-      <c r="S26" s="8"/>
-      <c r="V26" s="8"/>
+      <c r="D26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="S26" s="11"/>
+      <c r="V26" s="11"/>
     </row>
     <row r="27">
       <c r="A27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="M27" s="8"/>
-      <c r="P27" s="8"/>
-      <c r="S27" s="8"/>
-      <c r="V27" s="8"/>
+      <c r="D27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="J27" s="11"/>
+      <c r="M27" s="11"/>
+      <c r="P27" s="11"/>
+      <c r="S27" s="11"/>
+      <c r="V27" s="11"/>
     </row>
     <row r="28">
       <c r="A28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="D28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="15" t="s">
+      <c r="D28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="J28" s="8"/>
-      <c r="M28" s="8"/>
-      <c r="N28" s="15" t="s">
+      <c r="J28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="P28" s="8"/>
-      <c r="S28" s="8"/>
-      <c r="V28" s="8"/>
+      <c r="P28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="V28" s="11"/>
     </row>
     <row r="29">
       <c r="A29" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="16"/>
-      <c r="D29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="16"/>
-      <c r="J29" s="8"/>
-      <c r="M29" s="8"/>
-      <c r="N29" s="16"/>
-      <c r="P29" s="8"/>
-      <c r="S29" s="8"/>
-      <c r="V29" s="8"/>
+      <c r="B29" s="18"/>
+      <c r="D29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="18"/>
+      <c r="J29" s="11"/>
+      <c r="M29" s="11"/>
+      <c r="N29" s="18"/>
+      <c r="P29" s="11"/>
+      <c r="S29" s="11"/>
+      <c r="V29" s="11"/>
     </row>
     <row r="30">
       <c r="A30" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="16"/>
-      <c r="D30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="16"/>
-      <c r="J30" s="8"/>
-      <c r="M30" s="8"/>
-      <c r="N30" s="16"/>
-      <c r="P30" s="8"/>
-      <c r="S30" s="8"/>
-      <c r="V30" s="8"/>
+      <c r="B30" s="18"/>
+      <c r="D30" s="11"/>
+      <c r="G30" s="11"/>
+      <c r="H30" s="18"/>
+      <c r="J30" s="11"/>
+      <c r="M30" s="11"/>
+      <c r="N30" s="18"/>
+      <c r="P30" s="11"/>
+      <c r="S30" s="11"/>
+      <c r="V30" s="11"/>
     </row>
     <row r="31">
       <c r="A31" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="17"/>
-      <c r="D31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="17"/>
-      <c r="J31" s="8"/>
-      <c r="M31" s="8"/>
-      <c r="N31" s="17"/>
-      <c r="P31" s="8"/>
-      <c r="S31" s="8"/>
-      <c r="V31" s="8"/>
+      <c r="B31" s="19"/>
+      <c r="D31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="19"/>
+      <c r="J31" s="11"/>
+      <c r="M31" s="11"/>
+      <c r="N31" s="19"/>
+      <c r="P31" s="11"/>
+      <c r="S31" s="11"/>
+      <c r="V31" s="11"/>
     </row>
     <row r="32">
       <c r="A32" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="M32" s="8"/>
-      <c r="P32" s="8"/>
-      <c r="S32" s="8"/>
-      <c r="V32" s="8"/>
+      <c r="D32" s="11"/>
+      <c r="G32" s="11"/>
+      <c r="J32" s="11"/>
+      <c r="M32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="V32" s="11"/>
     </row>
     <row r="33">
       <c r="A33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="M33" s="8"/>
-      <c r="P33" s="8"/>
-      <c r="S33" s="8"/>
-      <c r="V33" s="8"/>
+      <c r="D33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="J33" s="11"/>
+      <c r="M33" s="11"/>
+      <c r="P33" s="11"/>
+      <c r="S33" s="11"/>
+      <c r="V33" s="11"/>
     </row>
     <row r="34">
       <c r="A34" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="8"/>
-      <c r="G34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="M34" s="8"/>
-      <c r="P34" s="8"/>
-      <c r="S34" s="8"/>
-      <c r="V34" s="8"/>
+      <c r="D34" s="11"/>
+      <c r="G34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="P34" s="11"/>
+      <c r="S34" s="11"/>
+      <c r="V34" s="11"/>
     </row>
     <row r="35">
       <c r="A35" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="F35" s="23" t="s">
+      <c r="D35" s="11"/>
+      <c r="F35" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="V35" s="8"/>
+      <c r="G35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="V35" s="11"/>
     </row>
     <row r="36">
       <c r="A36" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="8"/>
-      <c r="F36" s="24"/>
-      <c r="G36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="M36" s="8"/>
-      <c r="P36" s="8"/>
-      <c r="S36" s="8"/>
-      <c r="V36" s="8"/>
+      <c r="D36" s="11"/>
+      <c r="F36" s="25"/>
+      <c r="G36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="M36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="S36" s="11"/>
+      <c r="V36" s="11"/>
     </row>
     <row r="37">
       <c r="A37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D37" s="8"/>
-      <c r="F37" s="24"/>
-      <c r="G37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="M37" s="8"/>
-      <c r="P37" s="8"/>
-      <c r="S37" s="8"/>
-      <c r="V37" s="8"/>
+      <c r="D37" s="11"/>
+      <c r="F37" s="25"/>
+      <c r="G37" s="11"/>
+      <c r="J37" s="11"/>
+      <c r="M37" s="11"/>
+      <c r="P37" s="11"/>
+      <c r="S37" s="11"/>
+      <c r="V37" s="11"/>
     </row>
     <row r="38">
       <c r="A38" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="8"/>
-      <c r="E38" s="15" t="s">
+      <c r="D38" s="11"/>
+      <c r="E38" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F38" s="25"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="15" t="s">
+      <c r="F38" s="26"/>
+      <c r="G38" s="11"/>
+      <c r="H38" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="J38" s="8"/>
-      <c r="K38" s="15" t="s">
+      <c r="J38" s="11"/>
+      <c r="K38" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="M38" s="8"/>
-      <c r="N38" s="15" t="s">
+      <c r="M38" s="11"/>
+      <c r="N38" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="P38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="V38" s="8"/>
+      <c r="P38" s="11"/>
+      <c r="S38" s="11"/>
+      <c r="V38" s="11"/>
     </row>
     <row r="39">
       <c r="A39" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D39" s="8"/>
-      <c r="E39" s="16"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="16"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="16"/>
-      <c r="M39" s="8"/>
-      <c r="N39" s="16"/>
-      <c r="P39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="V39" s="8"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="18"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="18"/>
+      <c r="J39" s="11"/>
+      <c r="K39" s="18"/>
+      <c r="M39" s="11"/>
+      <c r="N39" s="18"/>
+      <c r="P39" s="11"/>
+      <c r="S39" s="11"/>
+      <c r="V39" s="11"/>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D40" s="8"/>
-      <c r="E40" s="16"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="16"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="16"/>
-      <c r="M40" s="8"/>
-      <c r="N40" s="16"/>
-      <c r="P40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="V40" s="8"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="18"/>
+      <c r="G40" s="11"/>
+      <c r="H40" s="18"/>
+      <c r="J40" s="11"/>
+      <c r="K40" s="18"/>
+      <c r="M40" s="11"/>
+      <c r="N40" s="18"/>
+      <c r="P40" s="11"/>
+      <c r="S40" s="11"/>
+      <c r="V40" s="11"/>
     </row>
     <row r="41">
       <c r="A41" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="8"/>
-      <c r="E41" s="17"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="17"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="17"/>
-      <c r="M41" s="8"/>
-      <c r="N41" s="17"/>
-      <c r="P41" s="8"/>
-      <c r="S41" s="8"/>
-      <c r="V41" s="8"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="19"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="19"/>
+      <c r="J41" s="11"/>
+      <c r="K41" s="19"/>
+      <c r="M41" s="11"/>
+      <c r="N41" s="19"/>
+      <c r="P41" s="11"/>
+      <c r="S41" s="11"/>
+      <c r="V41" s="11"/>
     </row>
     <row r="42">
       <c r="A42" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="8"/>
-      <c r="G42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="M42" s="8"/>
-      <c r="P42" s="8"/>
-      <c r="S42" s="8"/>
-      <c r="V42" s="8"/>
+      <c r="D42" s="11"/>
+      <c r="G42" s="11"/>
+      <c r="J42" s="11"/>
+      <c r="M42" s="11"/>
+      <c r="P42" s="11"/>
+      <c r="S42" s="11"/>
+      <c r="V42" s="11"/>
     </row>
     <row r="43">
       <c r="A43" s="2" t="s">
@@ -1979,311 +2231,338 @@
       <c r="D43" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="G43" s="8"/>
+      <c r="G43" s="11"/>
       <c r="J43" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="M43" s="8"/>
+      <c r="M43" s="11"/>
       <c r="P43" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="S43" s="8"/>
-      <c r="V43" s="8"/>
+      <c r="S43" s="11"/>
+      <c r="V43" s="11"/>
     </row>
     <row r="44">
       <c r="A44" s="3" t="s">
         <v>22</v>
       </c>
       <c r="D44" s="29"/>
-      <c r="G44" s="8"/>
+      <c r="G44" s="11"/>
       <c r="J44" s="29"/>
-      <c r="M44" s="8"/>
+      <c r="M44" s="11"/>
       <c r="P44" s="29"/>
-      <c r="S44" s="8"/>
-      <c r="V44" s="8"/>
+      <c r="S44" s="11"/>
+      <c r="V44" s="11"/>
     </row>
     <row r="45">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="29"/>
-      <c r="G45" s="8"/>
+      <c r="G45" s="11"/>
       <c r="J45" s="29"/>
-      <c r="M45" s="8"/>
+      <c r="M45" s="11"/>
       <c r="P45" s="29"/>
-      <c r="S45" s="8"/>
-      <c r="V45" s="8"/>
+      <c r="S45" s="11"/>
+      <c r="V45" s="11"/>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
         <v>23</v>
       </c>
       <c r="D46" s="31"/>
-      <c r="G46" s="8"/>
+      <c r="G46" s="11"/>
       <c r="J46" s="31"/>
-      <c r="M46" s="8"/>
+      <c r="M46" s="11"/>
       <c r="P46" s="31"/>
-      <c r="S46" s="8"/>
-      <c r="V46" s="8"/>
+      <c r="S46" s="11"/>
+      <c r="V46" s="11"/>
     </row>
     <row r="47">
       <c r="A47" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="M47" s="8"/>
-      <c r="P47" s="8"/>
-      <c r="S47" s="8"/>
-      <c r="V47" s="8"/>
+      <c r="D47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="J47" s="11"/>
+      <c r="M47" s="11"/>
+      <c r="P47" s="11"/>
+      <c r="S47" s="11"/>
+      <c r="V47" s="11"/>
     </row>
     <row r="48">
       <c r="A48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="M48" s="8"/>
-      <c r="P48" s="8"/>
-      <c r="S48" s="8"/>
-      <c r="V48" s="8"/>
+      <c r="D48" s="11"/>
+      <c r="G48" s="11"/>
+      <c r="J48" s="11"/>
+      <c r="M48" s="11"/>
+      <c r="P48" s="11"/>
+      <c r="S48" s="11"/>
+      <c r="V48" s="11"/>
     </row>
     <row r="49">
       <c r="A49" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D49" s="8"/>
-      <c r="G49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="M49" s="8"/>
-      <c r="P49" s="8"/>
-      <c r="S49" s="8"/>
-      <c r="V49" s="8"/>
+      <c r="D49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="J49" s="11"/>
+      <c r="M49" s="11"/>
+      <c r="P49" s="11"/>
+      <c r="S49" s="11"/>
+      <c r="V49" s="11"/>
     </row>
     <row r="50">
       <c r="A50" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D50" s="8"/>
-      <c r="G50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="M50" s="8"/>
-      <c r="P50" s="8"/>
-      <c r="S50" s="8"/>
-      <c r="V50" s="8"/>
+      <c r="D50" s="11"/>
+      <c r="G50" s="11"/>
+      <c r="J50" s="11"/>
+      <c r="M50" s="11"/>
+      <c r="P50" s="11"/>
+      <c r="S50" s="11"/>
+      <c r="V50" s="11"/>
     </row>
     <row r="51">
       <c r="A51" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D51" s="8"/>
-      <c r="G51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="M51" s="8"/>
-      <c r="P51" s="8"/>
-      <c r="S51" s="8"/>
-      <c r="V51" s="8"/>
+      <c r="D51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="J51" s="11"/>
+      <c r="M51" s="11"/>
+      <c r="P51" s="11"/>
+      <c r="S51" s="11"/>
+      <c r="V51" s="11"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D52" s="8"/>
-      <c r="G52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="M52" s="8"/>
-      <c r="P52" s="8"/>
-      <c r="S52" s="8"/>
-      <c r="V52" s="8"/>
+      <c r="D52" s="11"/>
+      <c r="G52" s="11"/>
+      <c r="J52" s="11"/>
+      <c r="M52" s="11"/>
+      <c r="P52" s="11"/>
+      <c r="S52" s="11"/>
+      <c r="V52" s="11"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="8"/>
-      <c r="G53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="L53" s="23" t="s">
+      <c r="D53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="J53" s="11"/>
+      <c r="L53" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="M53" s="8"/>
-      <c r="P53" s="8"/>
-      <c r="S53" s="8"/>
-      <c r="V53" s="8"/>
+      <c r="M53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="S53" s="11"/>
+      <c r="V53" s="11"/>
     </row>
     <row r="54">
       <c r="A54" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D54" s="8"/>
-      <c r="G54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="L54" s="24"/>
+      <c r="D54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="J54" s="11"/>
+      <c r="L54" s="25"/>
       <c r="M54" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="P54" s="8"/>
-      <c r="S54" s="8"/>
-      <c r="V54" s="8"/>
+      <c r="P54" s="11"/>
+      <c r="S54" s="11"/>
+      <c r="V54" s="11"/>
     </row>
     <row r="55">
       <c r="A55" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D55" s="8"/>
-      <c r="G55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="L55" s="24"/>
+      <c r="D55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="J55" s="11"/>
+      <c r="L55" s="25"/>
       <c r="M55" s="29"/>
-      <c r="P55" s="8"/>
-      <c r="S55" s="8"/>
-      <c r="V55" s="8"/>
+      <c r="P55" s="11"/>
+      <c r="S55" s="11"/>
+      <c r="V55" s="11"/>
     </row>
     <row r="56">
       <c r="A56" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D56" s="8"/>
-      <c r="G56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="L56" s="24"/>
+      <c r="D56" s="11"/>
+      <c r="G56" s="11"/>
+      <c r="J56" s="11"/>
+      <c r="L56" s="25"/>
       <c r="M56" s="29"/>
-      <c r="P56" s="8"/>
-      <c r="S56" s="8"/>
-      <c r="V56" s="8"/>
+      <c r="P56" s="11"/>
+      <c r="S56" s="11"/>
+      <c r="V56" s="11"/>
     </row>
     <row r="57">
       <c r="A57" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D57" s="8"/>
-      <c r="G57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="L57" s="24"/>
+      <c r="D57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="J57" s="11"/>
+      <c r="L57" s="25"/>
       <c r="M57" s="29"/>
-      <c r="P57" s="8"/>
-      <c r="S57" s="8"/>
-      <c r="V57" s="8"/>
+      <c r="P57" s="11"/>
+      <c r="S57" s="11"/>
+      <c r="V57" s="11"/>
     </row>
     <row r="58">
       <c r="A58" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D58" s="8"/>
-      <c r="G58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="L58" s="24"/>
+      <c r="D58" s="11"/>
+      <c r="G58" s="11"/>
+      <c r="J58" s="11"/>
+      <c r="L58" s="25"/>
       <c r="M58" s="29"/>
-      <c r="P58" s="8"/>
-      <c r="S58" s="8"/>
-      <c r="V58" s="8"/>
+      <c r="P58" s="11"/>
+      <c r="S58" s="11"/>
+      <c r="V58" s="11"/>
     </row>
     <row r="59">
       <c r="A59" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D59" s="8"/>
-      <c r="G59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="L59" s="24"/>
+      <c r="D59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="L59" s="25"/>
       <c r="M59" s="29"/>
-      <c r="P59" s="8"/>
-      <c r="S59" s="8"/>
-      <c r="V59" s="8"/>
+      <c r="P59" s="11"/>
+      <c r="S59" s="11"/>
+      <c r="V59" s="11"/>
     </row>
     <row r="60">
       <c r="A60" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D60" s="8"/>
-      <c r="G60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="L60" s="24"/>
+      <c r="D60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="J60" s="11"/>
+      <c r="L60" s="25"/>
       <c r="M60" s="29"/>
-      <c r="P60" s="8"/>
-      <c r="S60" s="8"/>
-      <c r="V60" s="8"/>
+      <c r="P60" s="11"/>
+      <c r="S60" s="11"/>
+      <c r="V60" s="11"/>
     </row>
     <row r="61">
       <c r="A61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D61" s="8"/>
-      <c r="G61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="L61" s="24"/>
+      <c r="D61" s="11"/>
+      <c r="G61" s="11"/>
+      <c r="J61" s="11"/>
+      <c r="L61" s="25"/>
       <c r="M61" s="31"/>
-      <c r="P61" s="8"/>
-      <c r="S61" s="8"/>
-      <c r="V61" s="8"/>
+      <c r="P61" s="11"/>
+      <c r="S61" s="11"/>
+      <c r="V61" s="11"/>
     </row>
     <row r="62">
       <c r="A62" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D62" s="8"/>
-      <c r="G62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="L62" s="24"/>
-      <c r="M62" s="8"/>
-      <c r="P62" s="8"/>
-      <c r="S62" s="8"/>
-      <c r="V62" s="8"/>
+      <c r="D62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="J62" s="11"/>
+      <c r="L62" s="25"/>
+      <c r="M62" s="11"/>
+      <c r="P62" s="11"/>
+      <c r="S62" s="11"/>
+      <c r="V62" s="11"/>
     </row>
     <row r="63">
       <c r="A63" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D63" s="8"/>
-      <c r="G63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="L63" s="24"/>
-      <c r="M63" s="8"/>
-      <c r="P63" s="8"/>
-      <c r="S63" s="8"/>
-      <c r="V63" s="8"/>
+      <c r="D63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="J63" s="11"/>
+      <c r="L63" s="25"/>
+      <c r="M63" s="11"/>
+      <c r="P63" s="11"/>
+      <c r="S63" s="11"/>
+      <c r="V63" s="11"/>
     </row>
     <row r="64">
       <c r="A64" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D64" s="8"/>
-      <c r="G64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="L64" s="25"/>
-      <c r="M64" s="8"/>
-      <c r="P64" s="8"/>
-      <c r="S64" s="8"/>
-      <c r="V64" s="8"/>
+      <c r="D64" s="11"/>
+      <c r="G64" s="11"/>
+      <c r="J64" s="11"/>
+      <c r="L64" s="26"/>
+      <c r="M64" s="11"/>
+      <c r="P64" s="11"/>
+      <c r="S64" s="11"/>
+      <c r="V64" s="11"/>
     </row>
     <row r="65">
       <c r="A65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D65" s="8"/>
-      <c r="G65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="M65" s="8"/>
-      <c r="P65" s="8"/>
-      <c r="S65" s="8"/>
-      <c r="V65" s="8"/>
+      <c r="D65" s="11"/>
+      <c r="G65" s="11"/>
+      <c r="J65" s="11"/>
+      <c r="M65" s="11"/>
+      <c r="P65" s="11"/>
+      <c r="S65" s="11"/>
+      <c r="V65" s="11"/>
     </row>
     <row r="66">
       <c r="A66" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D66" s="8"/>
-      <c r="G66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="M66" s="8"/>
-      <c r="P66" s="8"/>
-      <c r="S66" s="8"/>
-      <c r="V66" s="8"/>
+      <c r="D66" s="11"/>
+      <c r="G66" s="11"/>
+      <c r="J66" s="11"/>
+      <c r="M66" s="11"/>
+      <c r="P66" s="11"/>
+      <c r="S66" s="11"/>
+      <c r="V66" s="11"/>
     </row>
     <row r="67">
-      <c r="A67"/>
+      <c r="A67" s="40"/>
+      <c r="B67" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="C67" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D67" s="39" t="s">
+        <v>52</v>
+      </c>
+      <c r="E67" s="36"/>
+      <c r="F67" s="36"/>
+      <c r="G67" s="36"/>
+      <c r="H67" s="36"/>
+      <c r="I67" s="36"/>
+      <c r="J67" s="36"/>
+      <c r="K67" s="36"/>
+      <c r="L67" s="36"/>
+      <c r="M67" s="36"/>
+      <c r="N67" s="36"/>
+      <c r="O67" s="36"/>
+      <c r="P67" s="36"/>
+      <c r="Q67" s="36"/>
+      <c r="R67" s="36"/>
+      <c r="S67" s="36"/>
+      <c r="T67" s="36"/>
+      <c r="U67" s="36"/>
+      <c r="V67" s="41"/>
     </row>
     <row r="68">
       <c r="A68"/>

</xml_diff>